<commit_message>
Heamaps for Author-Based Proximity measures
</commit_message>
<xml_diff>
--- a/xl_data/otero-phpmyadmin-authorProxmeasure.xlsx
+++ b/xl_data/otero-phpmyadmin-authorProxmeasure.xlsx
@@ -1,40 +1,118 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\damon\COFC\bad-author\xl_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD02F73-0BE3-4614-97CA-5FB3767A915F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-15555" yWindow="7305" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="phpmyadmin" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="phpmyadmin" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+  <si>
+    <t>Bug_Rule</t>
+  </si>
+  <si>
+    <t>V-php:S2068</t>
+  </si>
+  <si>
+    <t>php:S905</t>
+  </si>
+  <si>
+    <t>javascript:S2259</t>
+  </si>
+  <si>
+    <t>php:S836</t>
+  </si>
+  <si>
+    <t>php:S2201</t>
+  </si>
+  <si>
+    <t>javascript:S2137</t>
+  </si>
+  <si>
+    <t>javascript:DuplicatePropertyName</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="2" tint="-9.9978637043366805E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -42,17 +120,72 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -340,134 +473,415 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A1:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="8" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Bug_Rule</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>V-php:S2068</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>V-php:S2068</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>V-php:S2068</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>V-php:S2068</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>V-php:S2068</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>V-php:S2068</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>V-php:S2068</t>
-        </is>
-      </c>
+    <row r="1" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1"/>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>php:S905</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3">
         <v>10</v>
       </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <f>SUM(B2:H2)</f>
+        <v>10</v>
+      </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>javascript:S2259</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3">
         <v>560</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" s="3">
         <v>3</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" s="3">
         <v>30</v>
       </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <f t="shared" ref="I3:I8" si="0">SUM(B3:H3)</f>
+        <v>593</v>
+      </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>php:S836</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3">
         <v>10</v>
       </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>php:S2201</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3">
         <v>20</v>
       </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>javascript:S2137</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
         <v>1</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6" s="3">
         <v>10</v>
       </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>javascript:DuplicatePropertyName</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
         <v>2</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" s="3">
         <v>20</v>
       </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="4">
+        <f>SUM(B1:B7)</f>
+        <v>600</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" ref="C8:H8" si="1">SUM(C1:C7)</f>
+        <v>6</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="1"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <conditionalFormatting sqref="B2:H7">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="99"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFBE4102"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFA1C993"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFBE4102"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF92D050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFC00000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:H8">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="20"/>
+        <cfvo type="percentile" val="95"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFBE4102"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFA1C993"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFBE4102"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF92D050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFC00000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I7">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="20"/>
+        <cfvo type="percentile" val="95"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFBE4102"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFA1C993"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFBE4102"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF92D050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFC00000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>